<commit_message>
[김정우] 배틀 가능. - 몬스터, 캐릭터 ID를 0부터 시작하게 변경하였습니다. - ChapterInfoSheet에서 EnemyIds, FrontIds, BackIds는 1,2,3,4 와 같은 형식을 지켜야합니다. - ChapterInfoSheet에서 EnemyIds의 갯수와 FrontIds, BackIds의 갯수의 합이 같아야합니다. 예) EnemyIds 1, 2, 3 FrontIds 1 BackIds 1, 2
</commit_message>
<xml_diff>
--- a/Assets/Shared/ExcelImporter/Excels/ChapterInfoDataSheet.xlsx
+++ b/Assets/Shared/ExcelImporter/Excels/ChapterInfoDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\SynergyDungeon\Assets\Shared\ExcelImporter\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AAE01A-BD9C-45B3-830F-7DF5910628CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49459CB-3177-4C42-B751-E097BCFCCACD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="135" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3045" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChapterInfoDatas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="16">
   <si>
     <t>ChapterId</t>
   </si>
@@ -43,13 +43,6 @@
     <t>BackIds</t>
   </si>
   <si>
-    <t>5,6,7</t>
-  </si>
-  <si>
-    <t>MonsterIds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>1,1,1,1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -59,6 +52,29 @@
   </si>
   <si>
     <t>2,3,4,5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyIds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>1,3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,6</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -395,7 +411,7 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -425,7 +441,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -451,13 +467,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -495,9 +511,11 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
       <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
@@ -537,13 +555,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
       <c r="H4" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -581,13 +599,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -625,13 +643,13 @@
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -669,13 +687,13 @@
         <v>1</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -713,13 +731,13 @@
         <v>1</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -757,13 +775,13 @@
         <v>1</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -801,13 +819,13 @@
         <v>1</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -845,13 +863,13 @@
         <v>1</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
@@ -889,13 +907,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -933,13 +951,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -977,13 +995,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -1021,13 +1039,13 @@
         <v>1</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1065,13 +1083,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G16" s="13">
+        <v>1</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -1109,13 +1127,13 @@
         <v>1</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G17" s="13">
+        <v>1</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -1153,13 +1171,13 @@
         <v>1</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G18" s="13">
+        <v>1</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -1197,13 +1215,13 @@
         <v>1</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G19" s="13">
+        <v>1</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -1241,13 +1259,13 @@
         <v>1</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G20" s="15">
+        <v>1</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
@@ -1285,13 +1303,13 @@
         <v>1</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G21" s="15">
+        <v>1</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
@@ -1329,13 +1347,13 @@
         <v>1</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G22" s="15">
+        <v>1</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
@@ -1373,13 +1391,13 @@
         <v>1</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G23" s="15">
+        <v>1</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
@@ -1417,13 +1435,13 @@
         <v>1</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G24" s="15">
+        <v>1</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
@@ -1461,13 +1479,13 @@
         <v>1</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G25" s="17">
+        <v>1</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
@@ -1505,13 +1523,13 @@
         <v>1</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G26" s="17">
+        <v>1</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
@@ -1549,13 +1567,13 @@
         <v>1</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G27" s="17">
+        <v>1</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
@@ -1593,13 +1611,13 @@
         <v>1</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G28" s="17">
+        <v>1</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
@@ -1637,13 +1655,13 @@
         <v>1</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G29" s="17">
+        <v>1</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
@@ -1681,13 +1699,13 @@
         <v>1</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G30" s="19">
+        <v>1</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -1725,13 +1743,13 @@
         <v>1</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G31" s="19">
+        <v>1</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -1769,13 +1787,13 @@
         <v>1</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G32" s="19">
+        <v>1</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -1813,13 +1831,13 @@
         <v>1</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G33" s="19">
+        <v>1</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
@@ -1857,13 +1875,13 @@
         <v>1</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="G34" s="19">
+        <v>1</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>

</xml_diff>